<commit_message>
add feature for exp number and total quantity of same component
</commit_message>
<xml_diff>
--- a/Raw_Data/F037_For_PHA5021C.xlsx
+++ b/Raw_Data/F037_For_PHA5021C.xlsx
@@ -4,16 +4,16 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18520" windowHeight="7670" activeTab="2"/>
+    <workbookView windowWidth="19190" windowHeight="7670"/>
   </bookViews>
   <sheets>
-    <sheet name="Uncut Sheet" sheetId="3" r:id="rId1"/>
+    <sheet name="Uncut_Sheet" sheetId="3" r:id="rId1"/>
     <sheet name="Cassette" sheetId="2" r:id="rId2"/>
     <sheet name="Pipettes" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Cassette!$A$1:$H$42</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Uncut Sheet'!$A$1:$G$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Uncut_Sheet!$A$1:$G$42</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Pipettes!$A$1:$G$42</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="21">
   <si>
     <t>Doc. No</t>
   </si>
@@ -71,6 +71,15 @@
     <t>LOT NUMBER</t>
   </si>
   <si>
+    <t>15.08.2022</t>
+  </si>
+  <si>
+    <t>2024-07</t>
+  </si>
+  <si>
+    <t>16.08.2022</t>
+  </si>
+  <si>
     <t>Caps</t>
   </si>
   <si>
@@ -82,9 +91,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_-&quot;RM&quot;* #,##0_-;\-&quot;RM&quot;* #,##0_-;_-&quot;RM&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;RM&quot;* #,##0_-;\-&quot;RM&quot;* #,##0_-;_-&quot;RM&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_-&quot;RM&quot;* #,##0.00_-;\-&quot;RM&quot;* #,##0.00_-;_-&quot;RM&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="180" formatCode="dd\-mmm\-yy"/>
   </numFmts>
@@ -143,7 +152,45 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -151,7 +198,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -166,15 +213,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -196,24 +235,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -224,48 +250,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -280,7 +274,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -301,13 +310,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -319,121 +400,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -451,19 +430,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -475,13 +442,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -949,6 +958,63 @@
       <top/>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -968,15 +1034,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -994,54 +1051,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1053,148 +1062,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="42" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="43" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="40" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="42" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2404,8 +2413,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:C12"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="7"/>
@@ -2566,27 +2575,51 @@
       <c r="G13" s="38"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="35"/>
-      <c r="B14" s="36"/>
+      <c r="A14" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="36">
+        <v>115</v>
+      </c>
       <c r="C14" s="37"/>
-      <c r="D14" s="30"/>
+      <c r="D14" s="30">
+        <v>20</v>
+      </c>
       <c r="E14" s="31"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="38"/>
+      <c r="F14" s="33">
+        <f>B14-D14</f>
+        <v>95</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="35"/>
-      <c r="B15" s="36"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="30"/>
+      <c r="A15" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="36">
+        <f>F14</f>
+        <v>95</v>
+      </c>
+      <c r="C15" s="37"/>
+      <c r="D15" s="30">
+        <v>15</v>
+      </c>
       <c r="E15" s="31"/>
-      <c r="F15" s="33"/>
+      <c r="F15" s="33">
+        <f>B15-D15</f>
+        <v>80</v>
+      </c>
       <c r="G15" s="38"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="35"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="38"/>
+      <c r="B16" s="36">
+        <f>F15</f>
+        <v>80</v>
+      </c>
+      <c r="C16" s="37"/>
       <c r="D16" s="30"/>
       <c r="E16" s="31"/>
       <c r="F16" s="33"/>
@@ -3030,14 +3063,14 @@
         <v>9</v>
       </c>
       <c r="B10" s="45" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C10" s="46"/>
       <c r="D10" s="44" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="47" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F10" s="47"/>
       <c r="G10" s="44" t="s">
@@ -3433,7 +3466,7 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
process refactoring the output
</commit_message>
<xml_diff>
--- a/Raw_Data/F037_For_PHA5021C.xlsx
+++ b/Raw_Data/F037_For_PHA5021C.xlsx
@@ -4,26 +4,24 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19190" windowHeight="7670" activeTab="3"/>
+    <workbookView windowWidth="19190" windowHeight="7670" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Uncut_Sheet_1" sheetId="3" r:id="rId1"/>
-    <sheet name="Uncut_Sheet_2" sheetId="5" r:id="rId2"/>
-    <sheet name="Cassette_1" sheetId="2" r:id="rId3"/>
-    <sheet name="Pipettes_1" sheetId="4" r:id="rId4"/>
+    <sheet name="Cassette_1" sheetId="2" r:id="rId2"/>
+    <sheet name="Pipettes_1" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">Cassette_1!$A$1:$H$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Cassette_1!$A$1:$H$42</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Uncut_Sheet_1!$A$1:$G$42</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">Pipettes_1!$A$1:$G$42</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Uncut_Sheet_2!$A$1:$G$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">Pipettes_1!$A$1:$G$42</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
   <si>
     <t>Doc. No</t>
   </si>
@@ -93,10 +91,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_-&quot;RM&quot;* #,##0.00_-;\-&quot;RM&quot;* #,##0.00_-;_-&quot;RM&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;RM&quot;* #,##0_-;\-&quot;RM&quot;* #,##0_-;_-&quot;RM&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;RM&quot;* #,##0.00_-;\-&quot;RM&quot;* #,##0.00_-;_-&quot;RM&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;RM&quot;* #,##0_-;\-&quot;RM&quot;* #,##0_-;_-&quot;RM&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="180" formatCode="dd\-mmm\-yy"/>
   </numFmts>
   <fonts count="27">
@@ -154,21 +152,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -176,14 +159,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -197,8 +173,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -222,7 +206,68 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -236,64 +281,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -312,175 +310,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -496,6 +326,174 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="45">
     <border>
@@ -779,19 +777,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -965,19 +950,14 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -989,6 +969,69 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1008,204 +1051,159 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="43" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="40" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="42" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="42" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1310,6 +1308,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1319,16 +1320,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1338,6 +1333,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1351,31 +1349,28 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1383,16 +1378,16 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1405,6 +1400,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1746,235 +1744,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>981075</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2847975" y="47625"/>
-          <a:ext cx="3322320" cy="320675"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="en-US">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-            </a:defRPr>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-MY" sz="1800">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="7" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="7" charset="0"/>
-            </a:rPr>
-            <a:t>Raw</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-MY" sz="1800" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="7" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="7" charset="0"/>
-            </a:rPr>
-            <a:t> Material Stock Card</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-MY" sz="1800">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="7" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="7" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>85726</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>29322</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>765811</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>152512</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="85725" y="29210"/>
-          <a:ext cx="1766570" cy="307340"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -2155,7 +1924,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2789,7 +2558,7 @@
         <f>B12-D12</f>
         <v>0</v>
       </c>
-      <c r="G12" s="34" t="s">
+      <c r="G12" s="68" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2803,7 +2572,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="33"/>
-      <c r="G13" s="38"/>
+      <c r="G13" s="34"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="35" t="s">
@@ -2821,7 +2590,7 @@
         <f>B14-D14</f>
         <v>95</v>
       </c>
-      <c r="G14" s="38" t="s">
+      <c r="G14" s="34" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2842,7 +2611,7 @@
         <f>B15-D15</f>
         <v>80</v>
       </c>
-      <c r="G15" s="38" t="s">
+      <c r="G15" s="34" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2856,61 +2625,61 @@
       <c r="D16" s="30"/>
       <c r="E16" s="31"/>
       <c r="F16" s="33"/>
-      <c r="G16" s="38"/>
+      <c r="G16" s="34"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="35"/>
       <c r="B17" s="36"/>
-      <c r="C17" s="38"/>
+      <c r="C17" s="34"/>
       <c r="D17" s="30"/>
       <c r="E17" s="31"/>
       <c r="F17" s="33"/>
-      <c r="G17" s="38"/>
+      <c r="G17" s="34"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="35"/>
       <c r="B18" s="36"/>
-      <c r="C18" s="38"/>
+      <c r="C18" s="34"/>
       <c r="D18" s="30"/>
       <c r="E18" s="31"/>
       <c r="F18" s="33"/>
-      <c r="G18" s="38"/>
+      <c r="G18" s="34"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="35"/>
       <c r="B19" s="36"/>
-      <c r="C19" s="38"/>
+      <c r="C19" s="34"/>
       <c r="D19" s="30"/>
       <c r="E19" s="31"/>
       <c r="F19" s="33"/>
-      <c r="G19" s="38"/>
+      <c r="G19" s="34"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="35"/>
       <c r="B20" s="36"/>
-      <c r="C20" s="38"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="30"/>
       <c r="E20" s="31"/>
       <c r="F20" s="33"/>
-      <c r="G20" s="38"/>
+      <c r="G20" s="34"/>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="35"/>
       <c r="B21" s="36"/>
-      <c r="C21" s="38"/>
+      <c r="C21" s="34"/>
       <c r="D21" s="30"/>
       <c r="E21" s="31"/>
       <c r="F21" s="33"/>
-      <c r="G21" s="38"/>
+      <c r="G21" s="34"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="35"/>
       <c r="B22" s="36"/>
-      <c r="C22" s="38"/>
+      <c r="C22" s="34"/>
       <c r="D22" s="30"/>
       <c r="E22" s="31"/>
       <c r="F22" s="33"/>
-      <c r="G22" s="38"/>
+      <c r="G22" s="34"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="35"/>
@@ -2919,7 +2688,7 @@
       <c r="D23" s="30"/>
       <c r="E23" s="31"/>
       <c r="F23" s="33"/>
-      <c r="G23" s="38"/>
+      <c r="G23" s="34"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="35"/>
@@ -2928,7 +2697,7 @@
       <c r="D24" s="30"/>
       <c r="E24" s="31"/>
       <c r="F24" s="33"/>
-      <c r="G24" s="38"/>
+      <c r="G24" s="34"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="35"/>
@@ -2937,7 +2706,7 @@
       <c r="D25" s="30"/>
       <c r="E25" s="31"/>
       <c r="F25" s="33"/>
-      <c r="G25" s="38"/>
+      <c r="G25" s="34"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="35"/>
@@ -2946,7 +2715,7 @@
       <c r="D26" s="30"/>
       <c r="E26" s="31"/>
       <c r="F26" s="33"/>
-      <c r="G26" s="38"/>
+      <c r="G26" s="34"/>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="35"/>
@@ -2955,7 +2724,7 @@
       <c r="D27" s="30"/>
       <c r="E27" s="31"/>
       <c r="F27" s="33"/>
-      <c r="G27" s="38"/>
+      <c r="G27" s="34"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="35"/>
@@ -2964,7 +2733,7 @@
       <c r="D28" s="30"/>
       <c r="E28" s="31"/>
       <c r="F28" s="33"/>
-      <c r="G28" s="38"/>
+      <c r="G28" s="34"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="35"/>
@@ -2973,7 +2742,7 @@
       <c r="D29" s="30"/>
       <c r="E29" s="31"/>
       <c r="F29" s="33"/>
-      <c r="G29" s="38"/>
+      <c r="G29" s="34"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="35"/>
@@ -2982,7 +2751,7 @@
       <c r="D30" s="30"/>
       <c r="E30" s="31"/>
       <c r="F30" s="33"/>
-      <c r="G30" s="38"/>
+      <c r="G30" s="34"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="35"/>
@@ -2991,7 +2760,7 @@
       <c r="D31" s="30"/>
       <c r="E31" s="31"/>
       <c r="F31" s="33"/>
-      <c r="G31" s="38"/>
+      <c r="G31" s="34"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="35"/>
@@ -3000,7 +2769,7 @@
       <c r="D32" s="30"/>
       <c r="E32" s="31"/>
       <c r="F32" s="33"/>
-      <c r="G32" s="38"/>
+      <c r="G32" s="34"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="35"/>
@@ -3009,7 +2778,7 @@
       <c r="D33" s="30"/>
       <c r="E33" s="31"/>
       <c r="F33" s="33"/>
-      <c r="G33" s="38"/>
+      <c r="G33" s="34"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="35"/>
@@ -3018,7 +2787,7 @@
       <c r="D34" s="30"/>
       <c r="E34" s="31"/>
       <c r="F34" s="33"/>
-      <c r="G34" s="38"/>
+      <c r="G34" s="34"/>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="35"/>
@@ -3027,7 +2796,7 @@
       <c r="D35" s="30"/>
       <c r="E35" s="31"/>
       <c r="F35" s="33"/>
-      <c r="G35" s="38"/>
+      <c r="G35" s="34"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="35"/>
@@ -3036,7 +2805,7 @@
       <c r="D36" s="30"/>
       <c r="E36" s="31"/>
       <c r="F36" s="33"/>
-      <c r="G36" s="38"/>
+      <c r="G36" s="34"/>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="35"/>
@@ -3045,7 +2814,7 @@
       <c r="D37" s="30"/>
       <c r="E37" s="31"/>
       <c r="F37" s="33"/>
-      <c r="G37" s="38"/>
+      <c r="G37" s="34"/>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="35"/>
@@ -3054,7 +2823,7 @@
       <c r="D38" s="30"/>
       <c r="E38" s="31"/>
       <c r="F38" s="33"/>
-      <c r="G38" s="38"/>
+      <c r="G38" s="34"/>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="35"/>
@@ -3063,7 +2832,7 @@
       <c r="D39" s="30"/>
       <c r="E39" s="31"/>
       <c r="F39" s="33"/>
-      <c r="G39" s="38"/>
+      <c r="G39" s="34"/>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="35"/>
@@ -3072,7 +2841,7 @@
       <c r="D40" s="30"/>
       <c r="E40" s="31"/>
       <c r="F40" s="33"/>
-      <c r="G40" s="38"/>
+      <c r="G40" s="34"/>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="35"/>
@@ -3081,16 +2850,16 @@
       <c r="D41" s="30"/>
       <c r="E41" s="31"/>
       <c r="F41" s="33"/>
-      <c r="G41" s="38"/>
+      <c r="G41" s="34"/>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="35"/>
       <c r="B42" s="37"/>
       <c r="C42" s="37"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="40"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="39"/>
       <c r="F42" s="33"/>
-      <c r="G42" s="38"/>
+      <c r="G42" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="77">
@@ -3184,548 +2953,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="7"/>
-  <cols>
-    <col min="1" max="1" width="15.5545454545455" customWidth="1"/>
-    <col min="2" max="2" width="14.3363636363636" customWidth="1"/>
-    <col min="3" max="3" width="10.3363636363636" customWidth="1"/>
-    <col min="4" max="4" width="13.3363636363636" customWidth="1"/>
-    <col min="5" max="5" width="11.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="13.1090909090909" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7">
-        <v>41473</v>
-      </c>
-      <c r="G3" s="8"/>
-    </row>
-    <row r="4" ht="15.25"/>
-    <row r="5" spans="1:8">
-      <c r="A5" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="13"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="16"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="14"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="18"/>
-    </row>
-    <row r="8" ht="15.25" spans="1:7">
-      <c r="A8" s="19"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="23"/>
-    </row>
-    <row r="9" ht="15.25"/>
-    <row r="10" ht="16.5" customHeight="1" spans="1:7">
-      <c r="A10" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" ht="15.25" spans="1:7">
-      <c r="A11" s="27"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-    </row>
-    <row r="12" ht="15.5" spans="1:7">
-      <c r="A12" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="30">
-        <v>16</v>
-      </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="32">
-        <v>16</v>
-      </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="33">
-        <f t="shared" ref="F12:F15" si="0">B12-D12</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" ht="15.75" customHeight="1" spans="1:7">
-      <c r="A13" s="35"/>
-      <c r="B13" s="36">
-        <f t="shared" ref="B13:B16" si="1">F12</f>
-        <v>0</v>
-      </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="38"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="36">
-        <v>115</v>
-      </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="30">
-        <v>20</v>
-      </c>
-      <c r="E14" s="31"/>
-      <c r="F14" s="33">
-        <f t="shared" si="0"/>
-        <v>95</v>
-      </c>
-      <c r="G14" s="38" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="36">
-        <f t="shared" si="1"/>
-        <v>95</v>
-      </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="30">
-        <v>15</v>
-      </c>
-      <c r="E15" s="31"/>
-      <c r="F15" s="33">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="G15" s="38" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="35"/>
-      <c r="B16" s="36">
-        <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="38"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="35"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="38"/>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="35"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="38"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="35"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="38"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="35"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="38"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="35"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="38"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="35"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="38"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="35"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="38"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="35"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="38"/>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="35"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="38"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="35"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="38"/>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="35"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="38"/>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="35"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="38"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="35"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="38"/>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="35"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="38"/>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="35"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="38"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="35"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="38"/>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="35"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="38"/>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="35"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="38"/>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="35"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="38"/>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="35"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="38"/>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="35"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="38"/>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="35"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="38"/>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="35"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="38"/>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="35"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="38"/>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="35"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="38"/>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="35"/>
-      <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="40"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="38"/>
-    </row>
-  </sheetData>
-  <mergeCells count="77">
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="D10:E11"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="99" orientation="portrait"/>
-  <headerFooter/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:H42"/>
-  <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="7"/>
@@ -3743,31 +2972,31 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="43"/>
+      <c r="D3" s="42"/>
       <c r="E3" s="6" t="s">
         <v>2</v>
       </c>
@@ -3832,21 +3061,21 @@
     </row>
     <row r="9" ht="15.25"/>
     <row r="10" ht="16.5" customHeight="1" spans="1:8">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="44" t="s">
+      <c r="C10" s="45"/>
+      <c r="D10" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="47" t="s">
+      <c r="E10" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="47"/>
-      <c r="G10" s="44" t="s">
+      <c r="F10" s="46"/>
+      <c r="G10" s="43" t="s">
         <v>12</v>
       </c>
       <c r="H10" s="26" t="s">
@@ -3854,41 +3083,41 @@
       </c>
     </row>
     <row r="11" ht="15.25" spans="1:8">
-      <c r="A11" s="48"/>
-      <c r="B11" s="49" t="s">
+      <c r="A11" s="47"/>
+      <c r="B11" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="51" t="s">
+      <c r="D11" s="47"/>
+      <c r="E11" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="50" t="s">
+      <c r="F11" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="48"/>
+      <c r="G11" s="47"/>
       <c r="H11" s="28"/>
     </row>
     <row r="12" ht="15.5" spans="1:8">
       <c r="A12" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="52">
+      <c r="B12" s="51">
         <v>3016</v>
       </c>
-      <c r="C12" s="53">
+      <c r="C12" s="52">
         <v>1080</v>
       </c>
       <c r="D12" s="29">
         <f>B12-C12</f>
         <v>1936</v>
       </c>
-      <c r="E12" s="54">
+      <c r="E12" s="53">
         <v>4858</v>
       </c>
-      <c r="F12" s="55">
+      <c r="F12" s="54">
         <v>1080</v>
       </c>
       <c r="G12" s="29">
@@ -3896,314 +3125,314 @@
         <v>3778</v>
       </c>
       <c r="H12" s="34" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1" spans="1:8">
       <c r="A13" s="35"/>
-      <c r="B13" s="56">
+      <c r="B13" s="55">
         <f>D12</f>
         <v>1936</v>
       </c>
-      <c r="C13" s="57"/>
+      <c r="C13" s="56"/>
       <c r="D13" s="35"/>
-      <c r="E13" s="56">
+      <c r="E13" s="55">
         <f>G12</f>
         <v>3778</v>
       </c>
-      <c r="F13" s="58"/>
+      <c r="F13" s="57"/>
       <c r="G13" s="35"/>
-      <c r="H13" s="38"/>
+      <c r="H13" s="34"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="35"/>
-      <c r="B14" s="56"/>
-      <c r="C14" s="59"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="58"/>
       <c r="D14" s="35"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="58"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="57"/>
       <c r="G14" s="35"/>
-      <c r="H14" s="38"/>
+      <c r="H14" s="34"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="35"/>
-      <c r="B15" s="56"/>
-      <c r="C15" s="59"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="58"/>
       <c r="D15" s="35"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="58"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="57"/>
       <c r="G15" s="35"/>
-      <c r="H15" s="38"/>
+      <c r="H15" s="34"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="35"/>
-      <c r="B16" s="56"/>
-      <c r="C16" s="59"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="58"/>
       <c r="D16" s="35"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="58"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="57"/>
       <c r="G16" s="35"/>
-      <c r="H16" s="38"/>
+      <c r="H16" s="34"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="35"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="59"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="58"/>
       <c r="D17" s="35"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="58"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="57"/>
       <c r="G17" s="35"/>
-      <c r="H17" s="38"/>
+      <c r="H17" s="34"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="35"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="59"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="58"/>
       <c r="D18" s="35"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="58"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="57"/>
       <c r="G18" s="35"/>
-      <c r="H18" s="38"/>
+      <c r="H18" s="34"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="35"/>
-      <c r="B19" s="56"/>
-      <c r="C19" s="59"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="58"/>
       <c r="D19" s="35"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="58"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="57"/>
       <c r="G19" s="35"/>
-      <c r="H19" s="38"/>
+      <c r="H19" s="34"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="35"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="59"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="58"/>
       <c r="D20" s="35"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="58"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="57"/>
       <c r="G20" s="35"/>
-      <c r="H20" s="38"/>
+      <c r="H20" s="34"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="35"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="59"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="58"/>
       <c r="D21" s="35"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="58"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="57"/>
       <c r="G21" s="35"/>
-      <c r="H21" s="38"/>
+      <c r="H21" s="34"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="35"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="59"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="58"/>
       <c r="D22" s="35"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="58"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="57"/>
       <c r="G22" s="35"/>
-      <c r="H22" s="38"/>
+      <c r="H22" s="34"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="35"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="59"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="58"/>
       <c r="D23" s="35"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="58"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="57"/>
       <c r="G23" s="35"/>
-      <c r="H23" s="38"/>
+      <c r="H23" s="34"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="35"/>
-      <c r="B24" s="56"/>
-      <c r="C24" s="61"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="60"/>
       <c r="D24" s="35"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="58"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="57"/>
       <c r="G24" s="35"/>
-      <c r="H24" s="38"/>
+      <c r="H24" s="34"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="35"/>
-      <c r="B25" s="56"/>
-      <c r="C25" s="57"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="56"/>
       <c r="D25" s="35"/>
-      <c r="E25" s="63"/>
-      <c r="F25" s="58"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="57"/>
       <c r="G25" s="35"/>
-      <c r="H25" s="38"/>
+      <c r="H25" s="34"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="35"/>
-      <c r="B26" s="56"/>
-      <c r="C26" s="64"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="63"/>
       <c r="D26" s="35"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="58"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="57"/>
       <c r="G26" s="35"/>
-      <c r="H26" s="38"/>
+      <c r="H26" s="34"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="35"/>
-      <c r="B27" s="56"/>
-      <c r="C27" s="57"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="56"/>
       <c r="D27" s="35"/>
-      <c r="E27" s="66"/>
-      <c r="F27" s="58"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="57"/>
       <c r="G27" s="35"/>
-      <c r="H27" s="38"/>
+      <c r="H27" s="34"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="35"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="57"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="56"/>
       <c r="D28" s="35"/>
-      <c r="E28" s="66"/>
-      <c r="F28" s="58"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="57"/>
       <c r="G28" s="35"/>
-      <c r="H28" s="38"/>
+      <c r="H28" s="34"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="35"/>
-      <c r="B29" s="56"/>
-      <c r="C29" s="57"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="56"/>
       <c r="D29" s="35"/>
-      <c r="E29" s="66"/>
-      <c r="F29" s="58"/>
+      <c r="E29" s="65"/>
+      <c r="F29" s="57"/>
       <c r="G29" s="35"/>
-      <c r="H29" s="38"/>
+      <c r="H29" s="34"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="35"/>
-      <c r="B30" s="56"/>
-      <c r="C30" s="57"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="56"/>
       <c r="D30" s="35"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="58"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="57"/>
       <c r="G30" s="35"/>
-      <c r="H30" s="38"/>
+      <c r="H30" s="34"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="35"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="61"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="60"/>
       <c r="D31" s="35"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="58"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="57"/>
       <c r="G31" s="35"/>
-      <c r="H31" s="38"/>
+      <c r="H31" s="34"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="35"/>
-      <c r="B32" s="56"/>
-      <c r="C32" s="61"/>
+      <c r="B32" s="55"/>
+      <c r="C32" s="60"/>
       <c r="D32" s="35"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="58"/>
+      <c r="E32" s="66"/>
+      <c r="F32" s="57"/>
       <c r="G32" s="35"/>
-      <c r="H32" s="38"/>
+      <c r="H32" s="34"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="35"/>
-      <c r="B33" s="56"/>
-      <c r="C33" s="61"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="60"/>
       <c r="D33" s="35"/>
-      <c r="E33" s="67"/>
-      <c r="F33" s="58"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="57"/>
       <c r="G33" s="35"/>
-      <c r="H33" s="38"/>
+      <c r="H33" s="34"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="35"/>
-      <c r="B34" s="56"/>
-      <c r="C34" s="57"/>
+      <c r="B34" s="55"/>
+      <c r="C34" s="56"/>
       <c r="D34" s="35"/>
-      <c r="E34" s="68"/>
-      <c r="F34" s="58"/>
+      <c r="E34" s="67"/>
+      <c r="F34" s="57"/>
       <c r="G34" s="35"/>
-      <c r="H34" s="38"/>
+      <c r="H34" s="34"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="35"/>
-      <c r="B35" s="56"/>
-      <c r="C35" s="57"/>
+      <c r="B35" s="55"/>
+      <c r="C35" s="56"/>
       <c r="D35" s="35"/>
-      <c r="E35" s="68"/>
-      <c r="F35" s="58"/>
+      <c r="E35" s="67"/>
+      <c r="F35" s="57"/>
       <c r="G35" s="35"/>
-      <c r="H35" s="38"/>
+      <c r="H35" s="34"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="35"/>
-      <c r="B36" s="56"/>
-      <c r="C36" s="61"/>
+      <c r="B36" s="55"/>
+      <c r="C36" s="60"/>
       <c r="D36" s="35"/>
-      <c r="E36" s="68"/>
-      <c r="F36" s="58"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="57"/>
       <c r="G36" s="35"/>
-      <c r="H36" s="38"/>
+      <c r="H36" s="34"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="35"/>
-      <c r="B37" s="56"/>
-      <c r="C37" s="61"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="60"/>
       <c r="D37" s="35"/>
-      <c r="E37" s="68"/>
-      <c r="F37" s="58"/>
+      <c r="E37" s="67"/>
+      <c r="F37" s="57"/>
       <c r="G37" s="35"/>
-      <c r="H37" s="38"/>
+      <c r="H37" s="34"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="35"/>
-      <c r="B38" s="56"/>
-      <c r="C38" s="61"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="60"/>
       <c r="D38" s="35"/>
-      <c r="E38" s="68"/>
-      <c r="F38" s="58"/>
+      <c r="E38" s="67"/>
+      <c r="F38" s="57"/>
       <c r="G38" s="35"/>
-      <c r="H38" s="38"/>
+      <c r="H38" s="34"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="35"/>
-      <c r="B39" s="56"/>
-      <c r="C39" s="61"/>
+      <c r="B39" s="55"/>
+      <c r="C39" s="60"/>
       <c r="D39" s="35"/>
-      <c r="E39" s="68"/>
-      <c r="F39" s="58"/>
+      <c r="E39" s="67"/>
+      <c r="F39" s="57"/>
       <c r="G39" s="35"/>
-      <c r="H39" s="38"/>
+      <c r="H39" s="34"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="35"/>
-      <c r="B40" s="56"/>
-      <c r="C40" s="61"/>
+      <c r="B40" s="55"/>
+      <c r="C40" s="60"/>
       <c r="D40" s="35"/>
-      <c r="E40" s="68"/>
-      <c r="F40" s="58"/>
+      <c r="E40" s="67"/>
+      <c r="F40" s="57"/>
       <c r="G40" s="35"/>
-      <c r="H40" s="38"/>
+      <c r="H40" s="34"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="35"/>
-      <c r="B41" s="56"/>
-      <c r="C41" s="61"/>
+      <c r="B41" s="55"/>
+      <c r="C41" s="60"/>
       <c r="D41" s="35"/>
-      <c r="E41" s="68"/>
-      <c r="F41" s="58"/>
+      <c r="E41" s="67"/>
+      <c r="F41" s="57"/>
       <c r="G41" s="35"/>
-      <c r="H41" s="38"/>
+      <c r="H41" s="34"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="35"/>
-      <c r="B42" s="56"/>
-      <c r="C42" s="61"/>
+      <c r="B42" s="55"/>
+      <c r="C42" s="60"/>
       <c r="D42" s="35"/>
-      <c r="E42" s="68"/>
-      <c r="F42" s="58"/>
+      <c r="E42" s="67"/>
+      <c r="F42" s="57"/>
       <c r="G42" s="35"/>
-      <c r="H42" s="38"/>
+      <c r="H42" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -4234,13 +3463,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:G5"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="7"/>
@@ -4385,7 +3614,7 @@
         <v>5820</v>
       </c>
       <c r="G12" s="34" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1" spans="1:7">
@@ -4398,7 +3627,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="33"/>
-      <c r="G13" s="38"/>
+      <c r="G13" s="34"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="35"/>
@@ -4407,79 +3636,79 @@
       <c r="D14" s="30"/>
       <c r="E14" s="31"/>
       <c r="F14" s="33"/>
-      <c r="G14" s="38"/>
+      <c r="G14" s="34"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="35"/>
       <c r="B15" s="36"/>
-      <c r="C15" s="38"/>
+      <c r="C15" s="34"/>
       <c r="D15" s="30"/>
       <c r="E15" s="31"/>
       <c r="F15" s="33"/>
-      <c r="G15" s="38"/>
+      <c r="G15" s="34"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="35"/>
       <c r="B16" s="36"/>
-      <c r="C16" s="38"/>
+      <c r="C16" s="34"/>
       <c r="D16" s="30"/>
       <c r="E16" s="31"/>
       <c r="F16" s="33"/>
-      <c r="G16" s="38"/>
+      <c r="G16" s="34"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="35"/>
       <c r="B17" s="36"/>
-      <c r="C17" s="38"/>
+      <c r="C17" s="34"/>
       <c r="D17" s="30"/>
       <c r="E17" s="31"/>
       <c r="F17" s="33"/>
-      <c r="G17" s="38"/>
+      <c r="G17" s="34"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="35"/>
       <c r="B18" s="36"/>
-      <c r="C18" s="38"/>
+      <c r="C18" s="34"/>
       <c r="D18" s="30"/>
       <c r="E18" s="31"/>
       <c r="F18" s="33"/>
-      <c r="G18" s="38"/>
+      <c r="G18" s="34"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="35"/>
       <c r="B19" s="36"/>
-      <c r="C19" s="38"/>
+      <c r="C19" s="34"/>
       <c r="D19" s="30"/>
       <c r="E19" s="31"/>
       <c r="F19" s="33"/>
-      <c r="G19" s="38"/>
+      <c r="G19" s="34"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="35"/>
       <c r="B20" s="36"/>
-      <c r="C20" s="38"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="30"/>
       <c r="E20" s="31"/>
       <c r="F20" s="33"/>
-      <c r="G20" s="38"/>
+      <c r="G20" s="34"/>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="35"/>
       <c r="B21" s="36"/>
-      <c r="C21" s="38"/>
+      <c r="C21" s="34"/>
       <c r="D21" s="30"/>
       <c r="E21" s="31"/>
       <c r="F21" s="33"/>
-      <c r="G21" s="38"/>
+      <c r="G21" s="34"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="35"/>
       <c r="B22" s="36"/>
-      <c r="C22" s="38"/>
+      <c r="C22" s="34"/>
       <c r="D22" s="30"/>
       <c r="E22" s="31"/>
       <c r="F22" s="33"/>
-      <c r="G22" s="38"/>
+      <c r="G22" s="34"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="35"/>
@@ -4488,7 +3717,7 @@
       <c r="D23" s="30"/>
       <c r="E23" s="31"/>
       <c r="F23" s="33"/>
-      <c r="G23" s="38"/>
+      <c r="G23" s="34"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="35"/>
@@ -4497,7 +3726,7 @@
       <c r="D24" s="30"/>
       <c r="E24" s="31"/>
       <c r="F24" s="33"/>
-      <c r="G24" s="38"/>
+      <c r="G24" s="34"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="35"/>
@@ -4506,7 +3735,7 @@
       <c r="D25" s="30"/>
       <c r="E25" s="31"/>
       <c r="F25" s="33"/>
-      <c r="G25" s="38"/>
+      <c r="G25" s="34"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="35"/>
@@ -4515,7 +3744,7 @@
       <c r="D26" s="30"/>
       <c r="E26" s="31"/>
       <c r="F26" s="33"/>
-      <c r="G26" s="38"/>
+      <c r="G26" s="34"/>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="35"/>
@@ -4524,7 +3753,7 @@
       <c r="D27" s="30"/>
       <c r="E27" s="31"/>
       <c r="F27" s="33"/>
-      <c r="G27" s="38"/>
+      <c r="G27" s="34"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="35"/>
@@ -4533,7 +3762,7 @@
       <c r="D28" s="30"/>
       <c r="E28" s="31"/>
       <c r="F28" s="33"/>
-      <c r="G28" s="38"/>
+      <c r="G28" s="34"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="35"/>
@@ -4542,7 +3771,7 @@
       <c r="D29" s="30"/>
       <c r="E29" s="31"/>
       <c r="F29" s="33"/>
-      <c r="G29" s="38"/>
+      <c r="G29" s="34"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="35"/>
@@ -4551,7 +3780,7 @@
       <c r="D30" s="30"/>
       <c r="E30" s="31"/>
       <c r="F30" s="33"/>
-      <c r="G30" s="38"/>
+      <c r="G30" s="34"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="35"/>
@@ -4560,7 +3789,7 @@
       <c r="D31" s="30"/>
       <c r="E31" s="31"/>
       <c r="F31" s="33"/>
-      <c r="G31" s="38"/>
+      <c r="G31" s="34"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="35"/>
@@ -4569,7 +3798,7 @@
       <c r="D32" s="30"/>
       <c r="E32" s="31"/>
       <c r="F32" s="33"/>
-      <c r="G32" s="38"/>
+      <c r="G32" s="34"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="35"/>
@@ -4578,7 +3807,7 @@
       <c r="D33" s="30"/>
       <c r="E33" s="31"/>
       <c r="F33" s="33"/>
-      <c r="G33" s="38"/>
+      <c r="G33" s="34"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="35"/>
@@ -4587,7 +3816,7 @@
       <c r="D34" s="30"/>
       <c r="E34" s="31"/>
       <c r="F34" s="33"/>
-      <c r="G34" s="38"/>
+      <c r="G34" s="34"/>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="35"/>
@@ -4596,7 +3825,7 @@
       <c r="D35" s="30"/>
       <c r="E35" s="31"/>
       <c r="F35" s="33"/>
-      <c r="G35" s="38"/>
+      <c r="G35" s="34"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="35"/>
@@ -4605,7 +3834,7 @@
       <c r="D36" s="30"/>
       <c r="E36" s="31"/>
       <c r="F36" s="33"/>
-      <c r="G36" s="38"/>
+      <c r="G36" s="34"/>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="35"/>
@@ -4614,7 +3843,7 @@
       <c r="D37" s="30"/>
       <c r="E37" s="31"/>
       <c r="F37" s="33"/>
-      <c r="G37" s="38"/>
+      <c r="G37" s="34"/>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="35"/>
@@ -4623,7 +3852,7 @@
       <c r="D38" s="30"/>
       <c r="E38" s="31"/>
       <c r="F38" s="33"/>
-      <c r="G38" s="38"/>
+      <c r="G38" s="34"/>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="35"/>
@@ -4632,7 +3861,7 @@
       <c r="D39" s="30"/>
       <c r="E39" s="31"/>
       <c r="F39" s="33"/>
-      <c r="G39" s="38"/>
+      <c r="G39" s="34"/>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="35"/>
@@ -4641,7 +3870,7 @@
       <c r="D40" s="30"/>
       <c r="E40" s="31"/>
       <c r="F40" s="33"/>
-      <c r="G40" s="38"/>
+      <c r="G40" s="34"/>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="35"/>
@@ -4650,16 +3879,16 @@
       <c r="D41" s="30"/>
       <c r="E41" s="31"/>
       <c r="F41" s="33"/>
-      <c r="G41" s="38"/>
+      <c r="G41" s="34"/>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="35"/>
       <c r="B42" s="37"/>
       <c r="C42" s="37"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="40"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="39"/>
       <c r="F42" s="33"/>
-      <c r="G42" s="38"/>
+      <c r="G42" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="77">

</xml_diff>